<commit_message>
GDD en scrumlog edits
</commit_message>
<xml_diff>
--- a/Aanwezigheid/Presentie GL-G5.xlsx
+++ b/Aanwezigheid/Presentie GL-G5.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="49">
   <si>
     <t>Maandag</t>
   </si>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,7 +1142,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="32">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B104+B112+B120+B128+B136+B144+B152+B168+B160+B176</f>
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="L2" s="47">
         <f>C8+C16+C24+C32+C48+C56+C64+C72+C80+C88+C96+C104+C120+C128+C136+C144+C152+C160+C168+C176</f>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="M2" s="53">
         <f>L2/K2</f>
-        <v>0.73076923076923073</v>
+        <v>0.54285714285714282</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>18</v>
@@ -1190,11 +1190,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="48">
         <f>D8+D16+D24+D32+D48+D56+D64+D72+D80+D88+D96+D104+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M3" s="54">
         <f>L3/K2</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N3" s="43" t="s">
         <v>19</v>
@@ -1232,11 +1232,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="49">
         <f>E8+E16+E24+E32+E48+E56+E64+E72+E80+E88+E96+E104+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M4" s="55">
         <f>L4/K2</f>
-        <v>0.92307692307692313</v>
+        <v>0.74285714285714288</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>20</v>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="M5" s="56">
         <f>L5/K2</f>
-        <v>0.73076923076923073</v>
+        <v>0.54285714285714282</v>
       </c>
       <c r="N5" s="45" t="s">
         <v>21</v>
@@ -1316,11 +1316,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="51">
         <f>G8+G16+G24+G32+G48+G56+G64+G72+G80+G88+G96+G104+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M6" s="57">
         <f>L6/K2</f>
-        <v>0.84615384615384615</v>
+        <v>0.68571428571428572</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>22</v>
@@ -1358,11 +1358,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="52">
         <f>H8+H88+H24+H32+H48+H56+H64+H72+H80+H96+H104+H120+H128+H136+H144+H152+H160+H168+H176+H16</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M7" s="58">
         <f>L7/K2</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>23</v>
@@ -1407,11 +1407,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="38">
         <f>I8+I16+I24+I32+I48+I56+I64+I72+I80+I88+I96+I104+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M8" s="39">
         <f>L8/K2</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>24</v>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="M10" s="29">
         <f>SUM(M2:M9)</f>
-        <v>6.2307692307692308</v>
+        <v>4.9142857142857137</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1917,22 +1917,42 @@
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="5"/>
+      <c r="B27" s="10">
+        <v>4</v>
+      </c>
+      <c r="C27" s="34">
+        <v>0</v>
+      </c>
+      <c r="D27" s="35">
+        <v>4</v>
+      </c>
+      <c r="E27" s="35">
+        <v>4</v>
+      </c>
+      <c r="F27" s="35">
+        <v>0</v>
+      </c>
+      <c r="G27" s="35">
+        <v>4</v>
+      </c>
+      <c r="H27" s="35">
+        <v>4</v>
+      </c>
+      <c r="I27" s="36">
+        <v>4</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="10">
+        <v>6</v>
+      </c>
       <c r="C28" s="34"/>
       <c r="D28" s="35"/>
       <c r="E28" s="35"/>
@@ -1962,7 +1982,9 @@
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="10"/>
+      <c r="B30" s="10">
+        <v>4</v>
+      </c>
       <c r="C30" s="34"/>
       <c r="D30" s="35"/>
       <c r="E30" s="35"/>
@@ -1977,7 +1999,9 @@
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="9">
+        <v>4</v>
+      </c>
       <c r="C31" s="82"/>
       <c r="D31" s="80"/>
       <c r="E31" s="80"/>
@@ -1993,7 +2017,7 @@
         <v>5</v>
       </c>
       <c r="B32" s="32">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C32" s="76">
         <f t="shared" ref="C32:G32" si="3">SUM(C27:C31)</f>
@@ -2001,11 +2025,11 @@
       </c>
       <c r="D32" s="77">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E32" s="77">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F32" s="77">
         <f t="shared" si="3"/>
@@ -2013,15 +2037,15 @@
       </c>
       <c r="G32" s="77">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32" s="77">
         <f>SUM(H27:H31)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I32" s="77">
         <f>SUM(I27:I31)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J32" s="27"/>
       <c r="K32" s="10"/>

</xml_diff>

<commit_message>
Ingame menu work and Presentie
Overall Menu work to be done :
- Add sprites
- Fill the collection list
- Fix saving and loading of save files.
</commit_message>
<xml_diff>
--- a/Aanwezigheid/Presentie GL-G5.xlsx
+++ b/Aanwezigheid/Presentie GL-G5.xlsx
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:N176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,11 +1193,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="48">
         <f>D8+D16+D24+D32+D48+D56+D64+D72+D80+D88+D96+D104+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M3" s="54">
         <f>L3/K2</f>
-        <v>0.88571428571428568</v>
+        <v>0.94285714285714284</v>
       </c>
       <c r="N3" s="43" t="s">
         <v>19</v>
@@ -1235,11 +1235,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="49">
         <f>E8+E16+E24+E32+E48+E56+E64+E72+E80+E88+E96+E104+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="M4" s="55">
         <f>L4/K2</f>
-        <v>0.82857142857142863</v>
+        <v>0.88571428571428568</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>20</v>
@@ -1319,11 +1319,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="51">
         <f>G8+G16+G24+G32+G48+G56+G64+G72+G80+G88+G96+G104+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="M6" s="57">
         <f>L6/K2</f>
-        <v>0.77142857142857146</v>
+        <v>0.82857142857142863</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>22</v>
@@ -1361,11 +1361,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="52">
         <f>H8+H88+H24+H32+H48+H56+H64+H72+H80+H96+H104+H120+H128+H136+H144+H152+H160+H168+H176+H16</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="M7" s="58">
         <f>L7/K2</f>
-        <v>0.8</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>23</v>
@@ -1410,11 +1410,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="38">
         <f>I8+I16+I24+I32+I48+I56+I64+I72+I80+I88+I96+I104+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="M8" s="39">
         <f>L8/K2</f>
-        <v>0.8</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>24</v>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="M10" s="29">
         <f>SUM(M2:M9)</f>
-        <v>5.2571428571428571</v>
+        <v>5.5428571428571427</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2004,13 +2004,27 @@
       <c r="B30" s="10">
         <v>4</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="36"/>
+      <c r="C30" s="34">
+        <v>0</v>
+      </c>
+      <c r="D30" s="35">
+        <v>4</v>
+      </c>
+      <c r="E30" s="35">
+        <v>4</v>
+      </c>
+      <c r="F30" s="35">
+        <v>0</v>
+      </c>
+      <c r="G30" s="35">
+        <v>4</v>
+      </c>
+      <c r="H30" s="35">
+        <v>4</v>
+      </c>
+      <c r="I30" s="36">
+        <v>4</v>
+      </c>
       <c r="J30" s="5"/>
       <c r="K30" s="10"/>
     </row>
@@ -2044,11 +2058,11 @@
       </c>
       <c r="D32" s="77">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E32" s="77">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F32" s="77">
         <f t="shared" si="3"/>
@@ -2056,15 +2070,15 @@
       </c>
       <c r="G32" s="77">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H32" s="77">
         <f>SUM(H27:H31)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I32" s="77">
         <f>SUM(I27:I31)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J32" s="27"/>
       <c r="K32" s="10"/>

</xml_diff>

<commit_message>
Presentie en Shader work .
</commit_message>
<xml_diff>
--- a/Aanwezigheid/Presentie GL-G5.xlsx
+++ b/Aanwezigheid/Presentie GL-G5.xlsx
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1160,15 +1160,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="32">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B104+B112+B120+B128+B136+B144+B152+B168+B160+B176</f>
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="L2" s="47">
         <f>C8+C16+C24+C32+C48+C56+C64+C72+C80+C88+C96+C104+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M2" s="53">
         <f>L2/K2</f>
-        <v>0.3392857142857143</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>18</v>
@@ -1208,11 +1208,11 @@
       <c r="K3" s="10"/>
       <c r="L3" s="48">
         <f>D8+D16+D24+D32+D48+D56+D64+D72+D80+D88+D96+D104+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="M3" s="54">
         <f>L3/K2</f>
-        <v>0.9107142857142857</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="N3" s="43" t="s">
         <v>19</v>
@@ -1250,11 +1250,11 @@
       <c r="K4" s="10"/>
       <c r="L4" s="49">
         <f>E8+E16+E24+E32+E48+E56+E64+E72+E80+E88+E96+E104+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="M4" s="55">
         <f>L4/K2</f>
-        <v>0.875</v>
+        <v>0.85</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>20</v>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="M5" s="56">
         <f>L5/K2</f>
-        <v>0.41964285714285715</v>
+        <v>0.39166666666666666</v>
       </c>
       <c r="N5" s="45" t="s">
         <v>21</v>
@@ -1334,11 +1334,11 @@
       <c r="K6" s="10"/>
       <c r="L6" s="51">
         <f>G8+G16+G24+G32+G48+G56+G64+G72+G80+G88+G96+G104+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="M6" s="57">
         <f>L6/K2</f>
-        <v>0.8392857142857143</v>
+        <v>0.81666666666666665</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>22</v>
@@ -1376,11 +1376,11 @@
       <c r="K7" s="10"/>
       <c r="L7" s="52">
         <f>H8+H88+H24+H32+H48+H56+H64+H72+H80+H96+H104+H120+H128+H136+H144+H152+H160+H168+H176+H16</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M7" s="58">
         <f>L7/K2</f>
-        <v>0.8571428571428571</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>23</v>
@@ -1425,11 +1425,11 @@
       <c r="K8" s="10"/>
       <c r="L8" s="38">
         <f>I8+I16+I24+I32+I48+I56+I64+I72+I80+I88+I96+I104+I120+I128+I136+I144+I152+I160+I168+I176</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M8" s="39">
         <f>L8/K2</f>
-        <v>0.8571428571428571</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N8" s="41" t="s">
         <v>24</v>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="M10" s="29">
         <f>SUM(M2:M9)</f>
-        <v>5.0982142857142856</v>
+        <v>4.9416666666666655</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2434,7 +2434,9 @@
       <c r="B46" s="10">
         <v>4</v>
       </c>
-      <c r="C46" s="34"/>
+      <c r="C46" s="34">
+        <v>2</v>
+      </c>
       <c r="D46" s="35">
         <v>4</v>
       </c>
@@ -2490,7 +2492,7 @@
       </c>
       <c r="C48" s="76">
         <f t="shared" ref="C48:G48" si="5">SUM(C43:C47)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D48" s="77">
         <f t="shared" si="5"/>
@@ -2786,12 +2788,22 @@
         <v>4</v>
       </c>
       <c r="C63" s="82"/>
-      <c r="D63" s="80"/>
-      <c r="E63" s="80"/>
+      <c r="D63" s="80">
+        <v>4</v>
+      </c>
+      <c r="E63" s="80">
+        <v>4</v>
+      </c>
       <c r="F63" s="80"/>
-      <c r="G63" s="80"/>
-      <c r="H63" s="80"/>
-      <c r="I63" s="81"/>
+      <c r="G63" s="80">
+        <v>4</v>
+      </c>
+      <c r="H63" s="80">
+        <v>4</v>
+      </c>
+      <c r="I63" s="81">
+        <v>4</v>
+      </c>
       <c r="J63" s="3"/>
       <c r="K63" s="10"/>
     </row>
@@ -2800,7 +2812,7 @@
         <v>5</v>
       </c>
       <c r="B64" s="32">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C64" s="76">
         <f t="shared" ref="C64:G64" si="7">SUM(C59:C63)</f>
@@ -2808,11 +2820,11 @@
       </c>
       <c r="D64" s="77">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E64" s="77">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F64" s="77">
         <f t="shared" si="7"/>
@@ -2820,15 +2832,15 @@
       </c>
       <c r="G64" s="77">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H64" s="77">
         <f>SUM(H59:H63)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I64" s="78">
         <f>SUM(I59:I63)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J64" s="31"/>
     </row>

</xml_diff>